<commit_message>
Admit card changes by stalin on 05-07-2023
</commit_message>
<xml_diff>
--- a/dataentry/uploaded_excel_files/cgle_2022_tier1.xlsx
+++ b/dataentry/uploaded_excel_files/cgle_2022_tier1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="197">
   <si>
     <t>ac_main_title</t>
   </si>
@@ -596,24 +596,6 @@
     <t>gateclose_p6</t>
   </si>
   <si>
-    <t>02-07-2023</t>
-  </si>
-  <si>
-    <t>03-07-2023</t>
-  </si>
-  <si>
-    <t>04-07-2023</t>
-  </si>
-  <si>
-    <t>05-07-2023</t>
-  </si>
-  <si>
-    <t>06-07-2023</t>
-  </si>
-  <si>
-    <t>07-07-2023</t>
-  </si>
-  <si>
     <t>08-07-2023</t>
   </si>
   <si>
@@ -621,6 +603,12 @@
   </si>
   <si>
     <t>scribe_opted_medium</t>
+  </si>
+  <si>
+    <t>10-07-2023</t>
+  </si>
+  <si>
+    <t>Yes (Own)</t>
   </si>
 </sst>
 </file>
@@ -966,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BT30"/>
+  <dimension ref="A1:BT31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -999,36 +987,28 @@
     <col min="26" max="26" width="10.85546875" customWidth="1"/>
     <col min="27" max="27" width="16" customWidth="1"/>
     <col min="28" max="28" width="8.140625" customWidth="1"/>
-    <col min="29" max="31" width="6.7109375" customWidth="1"/>
-    <col min="32" max="32" width="15.140625" customWidth="1"/>
+    <col min="29" max="32" width="6.7109375" customWidth="1"/>
     <col min="33" max="33" width="8.140625" customWidth="1"/>
     <col min="34" max="34" width="10.85546875" customWidth="1"/>
     <col min="35" max="35" width="6.7109375" customWidth="1"/>
     <col min="36" max="36" width="8.140625" customWidth="1"/>
-    <col min="37" max="39" width="6.7109375" customWidth="1"/>
-    <col min="40" max="40" width="16.140625" customWidth="1"/>
+    <col min="37" max="40" width="6.7109375" customWidth="1"/>
     <col min="41" max="41" width="8.140625" customWidth="1"/>
     <col min="42" max="42" width="10.85546875" customWidth="1"/>
     <col min="43" max="43" width="6.7109375" customWidth="1"/>
     <col min="44" max="44" width="8.140625" customWidth="1"/>
-    <col min="45" max="46" width="6.7109375" customWidth="1"/>
-    <col min="47" max="47" width="17.7109375" customWidth="1"/>
-    <col min="48" max="48" width="22.28515625" customWidth="1"/>
+    <col min="45" max="48" width="6.7109375" customWidth="1"/>
     <col min="49" max="49" width="12.140625" customWidth="1"/>
     <col min="50" max="50" width="8.140625" customWidth="1"/>
     <col min="51" max="51" width="10.85546875" customWidth="1"/>
     <col min="52" max="52" width="6.7109375" customWidth="1"/>
     <col min="53" max="53" width="8.140625" customWidth="1"/>
-    <col min="54" max="55" width="6.7109375" customWidth="1"/>
-    <col min="56" max="56" width="19.42578125" customWidth="1"/>
-    <col min="57" max="57" width="20.28515625" customWidth="1"/>
+    <col min="54" max="57" width="6.7109375" customWidth="1"/>
     <col min="58" max="58" width="8.140625" customWidth="1"/>
     <col min="59" max="59" width="10.85546875" customWidth="1"/>
     <col min="60" max="60" width="6.7109375" customWidth="1"/>
     <col min="61" max="61" width="8.140625" customWidth="1"/>
-    <col min="62" max="63" width="6.7109375" customWidth="1"/>
-    <col min="64" max="64" width="15.42578125" customWidth="1"/>
-    <col min="65" max="65" width="15.140625" customWidth="1"/>
+    <col min="62" max="65" width="6.7109375" customWidth="1"/>
     <col min="66" max="66" width="14.28515625" customWidth="1"/>
     <col min="67" max="67" width="14.140625" customWidth="1"/>
     <col min="68" max="68" width="13.42578125" customWidth="1"/>
@@ -1054,7 +1034,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1264,6 +1244,9 @@
       <c r="D2" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>86</v>
       </c>
@@ -1561,7 +1544,7 @@
         <v>172</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T6" s="4" t="s">
         <v>154</v>
@@ -1697,7 +1680,7 @@
         <v>172</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="T8" s="4" t="s">
         <v>154</v>
@@ -1765,7 +1748,7 @@
         <v>172</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="T9" s="4" t="s">
         <v>154</v>
@@ -1833,7 +1816,7 @@
         <v>172</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="T10" s="4" t="s">
         <v>154</v>
@@ -1901,7 +1884,7 @@
         <v>172</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="T11" s="4" t="s">
         <v>154</v>
@@ -1969,7 +1952,7 @@
         <v>172</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="T12" s="4" t="s">
         <v>154</v>
@@ -2037,7 +2020,7 @@
         <v>172</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="T13" s="4" t="s">
         <v>154</v>
@@ -2105,7 +2088,7 @@
         <v>172</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="T14" s="4" t="s">
         <v>154</v>
@@ -2173,7 +2156,7 @@
         <v>172</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="T15" s="4" t="s">
         <v>154</v>
@@ -2241,7 +2224,7 @@
         <v>172</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="T16" s="4" t="s">
         <v>154</v>
@@ -2309,7 +2292,7 @@
         <v>172</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="T17" s="4" t="s">
         <v>154</v>
@@ -2377,7 +2360,7 @@
         <v>172</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T18" s="4" t="s">
         <v>154</v>
@@ -2445,7 +2428,7 @@
         <v>172</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T19" s="4" t="s">
         <v>154</v>
@@ -2513,7 +2496,7 @@
         <v>172</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="T20" s="4" t="s">
         <v>154</v>
@@ -2581,7 +2564,7 @@
         <v>172</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="T21" s="4" t="s">
         <v>154</v>
@@ -2649,7 +2632,7 @@
         <v>172</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="T22" s="4" t="s">
         <v>154</v>
@@ -2717,7 +2700,7 @@
         <v>172</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="T23" s="4" t="s">
         <v>154</v>
@@ -2785,7 +2768,7 @@
         <v>172</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="T24" s="4" t="s">
         <v>154</v>
@@ -2853,7 +2836,7 @@
         <v>172</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>154</v>
@@ -2989,7 +2972,7 @@
         <v>172</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>154</v>
@@ -3057,7 +3040,7 @@
         <v>172</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>154</v>
@@ -3125,7 +3108,7 @@
         <v>172</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="T29" s="4" t="s">
         <v>154</v>
@@ -3193,7 +3176,7 @@
         <v>172</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="T30" s="4" t="s">
         <v>154</v>
@@ -3222,6 +3205,9 @@
       <c r="BR30" s="4" t="s">
         <v>175</v>
       </c>
+    </row>
+    <row r="31" spans="1:70">
+      <c r="S31" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>